<commit_message>
minor spacing cleanups only
</commit_message>
<xml_diff>
--- a/api-list.xlsx
+++ b/api-list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\wwwroot\apache\laravel\FreeVisaFreeTicket\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E76F8512-44F9-4894-AE18-7DE72457AC15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB1AC9BF-A410-44A2-80C7-557249477B49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{A596C150-A067-45A9-A0F7-661F4452AD61}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Method</t>
   </si>
@@ -65,19 +65,43 @@
   </si>
   <si>
     <t>email,password</t>
+  </si>
+  <si>
+    <t>candidate/job/home</t>
+  </si>
+  <si>
+    <t>GET</t>
+  </si>
+  <si>
+    <t>candidate/job-list</t>
+  </si>
+  <si>
+    <t>candidate/job-categories</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF212121"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFA31515"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -100,8 +124,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -416,17 +444,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AB43095-181B-46F5-96BE-0D991C0FA4DD}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34" customWidth="1"/>
     <col min="4" max="4" width="43.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -466,6 +494,24 @@
         <v>8</v>
       </c>
     </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C8" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>

<commit_message>
- fixed country flag url
</commit_message>
<xml_diff>
--- a/api-list.xlsx
+++ b/api-list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\wwwroot\apache\laravel\FreeVisaFreeTicket\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB1AC9BF-A410-44A2-80C7-557249477B49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C8AFA8E-F4DE-473C-AAC2-42F24A6170B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{A596C150-A067-45A9-A0F7-661F4452AD61}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
   <si>
     <t>Method</t>
   </si>
@@ -77,6 +77,30 @@
   </si>
   <si>
     <t>candidate/job-categories</t>
+  </si>
+  <si>
+    <t>POST</t>
+  </si>
+  <si>
+    <t>candidate/job/apply</t>
+  </si>
+  <si>
+    <t>job_id</t>
+  </si>
+  <si>
+    <t>candidate/job/apply/list</t>
+  </si>
+  <si>
+    <t>candidate/banners</t>
+  </si>
+  <si>
+    <t>candidate/news</t>
+  </si>
+  <si>
+    <t>candidate/news-categories</t>
+  </si>
+  <si>
+    <t>candidate/news/{id}</t>
   </si>
 </sst>
 </file>
@@ -444,10 +468,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AB43095-181B-46F5-96BE-0D991C0FA4DD}">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -512,6 +536,51 @@
         <v>13</v>
       </c>
     </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C9" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C10" s="2"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C15" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C16" t="s">
+        <v>21</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>